<commit_message>
initial code for keyword driven framework
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/keyword1/scenarios/open_scenarios.xlsx
+++ b/src/main/java/com/qa/keyword1/scenarios/open_scenarios.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bhpanchal\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bhpanchal\OneDrive - MMI HOLDINGS LTD\Documents\Workspace\KeywordDriverOpen\src\main\java\com\qa\keyword1\scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{364B8EFE-1839-464B-8FE2-F7E16C90916C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF60550-2661-47EE-96FE-E79AF3757914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12540" yWindow="5250" windowWidth="21600" windowHeight="11265" xr2:uid="{3EC26296-2D73-4BE9-8AEF-C0DFBF8B80BD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3EC26296-2D73-4BE9-8AEF-C0DFBF8B80BD}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -34,14 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="28">
   <si>
     <t>test step</t>
   </si>
   <si>
-    <t>locator</t>
-  </si>
-  <si>
     <t>action</t>
   </si>
   <si>
@@ -90,18 +87,6 @@
     <t>quit</t>
   </si>
   <si>
-    <t>id=Form_submitForm_FirstName</t>
-  </si>
-  <si>
-    <t>id=Form_submitForm_LastName</t>
-  </si>
-  <si>
-    <t>id=Form_submitForm_action_request</t>
-  </si>
-  <si>
-    <t>linkText=Contact Sales</t>
-  </si>
-  <si>
     <t>bhavin</t>
   </si>
   <si>
@@ -109,6 +94,30 @@
   </si>
   <si>
     <t>https://www.orangehrm.com/hris-hr-software-demo/</t>
+  </si>
+  <si>
+    <t>Form_submitForm_FirstName</t>
+  </si>
+  <si>
+    <t>Form_submitForm_LastName</t>
+  </si>
+  <si>
+    <t>Form_submitForm_action_request</t>
+  </si>
+  <si>
+    <t>Contact Sales</t>
+  </si>
+  <si>
+    <t>linkText</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>locatorType</t>
+  </si>
+  <si>
+    <t>locatorValue</t>
   </si>
 </sst>
 </file>
@@ -472,180 +481,216 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1173B199-3DEE-4C33-8AE0-DCDF0E1834A3}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
       <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="2" t="s">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
         <v>16</v>
       </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{734448D3-C1F5-497A-A311-DCA358CEA67A}"/>
-    <hyperlink ref="D9" r:id="rId2" xr:uid="{2D23F7F3-248D-427B-936A-163725FEA0E8}"/>
+    <hyperlink ref="E3" r:id="rId1" xr:uid="{734448D3-C1F5-497A-A311-DCA358CEA67A}"/>
+    <hyperlink ref="E9" r:id="rId2" xr:uid="{2D23F7F3-248D-427B-936A-163725FEA0E8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>